<commit_message>
CDS changes as of 02/13
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC02_CDS_phs002371_Gender_NotReported.xlsx
+++ b/InputFiles/CDS/TC02_CDS_phs002371_Gender_NotReported.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0925\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6700C7EA-E8C1-4F28-94AF-3F9EE4CB3F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62237592-4433-47D2-9B72-8A9ADFD5AC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -57,6 +57,108 @@
     <t>TsvExcel</t>
   </si>
   <si>
+    <t>TC02_CDS_phs002371_Gender_NotReported_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>TC02_CDS_phs002371_Gender_NotReported_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>SELECT
+    COUNT(DISTINCT s.study_name) AS "Studies",
+    COUNT(DISTINCT sp.participant_id) AS "Participants",
+    COUNT(DISTINCT smp.sample_id) AS "Samples",
+    COUNT(DISTINCT f.file_id) AS "Files"
+FROM 
+    df_participant sp
+JOIN 
+    df_study s ON sp."study.phs_accession" = s.phs_accession
+JOIN 
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+JOIN 
+    df_program p ON p.program_acronym = s."program.program_acronym"
+JOIN 
+    df_file f ON f."sample.sample_id" = smp.sample_id
+JOIN 
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+JOIN 
+    df_genomic_info gi ON gi."file.file_id" = f.file_id
+WHERE 
+    s.phs_accession = 'phs002371' AND sp.gender = 'Not Reported';</t>
+  </si>
+  <si>
+    <t>SELECT
+    DISTINCT (smp.sample_id) AS "Sample ID",
+    sp.participant_id AS "Participant ID", 
+    s.study_name AS "Study Name",
+    s.phs_accession AS Accession
+FROM 
+    df_participant sp
+JOIN 
+    df_study s ON sp."study.phs_accession" = s.phs_accession
+JOIN 
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+JOIN
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+JOIN
+    df_program p ON p.program_acronym = s."program.program_acronym"
+JOIN
+    df_file f1 ON f1."sample.sample_id" = smp.sample_id
+JOIN
+    df_genomic_info gi ON gi."file.file_id" = f1.file_id
+WHERE 
+    s.phs_accession = 'phs002371' AND sp.gender = 'Not Reported'
+ORDER BY 
+    smp.sample_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
+    f1.file_name AS "File Name",
+    s.study_name AS "Study Name",
+    s.phs_accession AS "Accession",
+    sp.participant_id AS "Participant Id",
+    COALESCE((
+        SELECT
+            REPLACE(GROUP_CONCAT(CASE WHEN rn &lt;= 5 THEN smp.sample_id ELSE NULL END, ', '), ', , ', ', ') ||
+            CASE WHEN MAX(rn) &gt; 5 THEN ', ...' ELSE '' END
+        FROM (
+            SELECT
+                smp.sample_id,
+                ROW_NUMBER() OVER (ORDER BY smp.sample_id) AS rn
+            FROM df_sample smp
+            WHERE smp."participant.study_participant_id" = sp.study_participant_id
+        ) smp
+    ), '') AS "Sample Id",
+    f1.file_type AS "File Type",
+    gi.library_strategy AS "Library Strategy"
+FROM 
+    df_study s
+INNER JOIN 
+    df_participant sp ON sp."study.phs_accession" = s.phs_accession
+INNER JOIN  
+    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN 
+    df_file f1 ON f1."sample.sample_id" = smp.sample_id
+INNER JOIN
+    df_genomic_info gi ON gi."file.file_id" = f1.file_id
+INNER JOIN
+    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
+INNER JOIN
+    df_program p ON p.program_acronym = s."program.program_acronym"
+WHERE 
+    s.phs_accession = 'phs002371' AND sp.gender = 'Not Reported'
+GROUP BY
+    f1.file_name,
+    s.study_name,
+    s.phs_accession,
+    sp.participant_id,
+    f1.file_type,
+    gi.library_strategy
+ORDER BY 
+    f1.file_name ASC
+LIMIT 100;</t>
+  </si>
+  <si>
     <t>WITH Distinct_Samples AS (
     SELECT DISTINCT
         sp.participant_id,
@@ -80,7 +182,7 @@
     JOIN
         df_genomic_info gi ON gi."file.file_id" = f1.file_id
     WHERE 
-        s.phs_accession = 'phs001287' AND sp.gender = 'Female'
+        s.phs_accession = 'phs002371' AND sp.gender = 'Not Reported'
 ),
 Sample_Limit AS (
     SELECT
@@ -116,110 +218,6 @@
     phs_accession,
     gender
 LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
-    DISTINCT (smp.sample_id) AS "Sample ID",
-    sp.participant_id AS "Participant ID", 
-    s.study_name AS "Study Name",
-    s.phs_accession AS Accession,
-    smp.sample_tumor_status AS Tumor,
-    smp.sample_type AS "Analyte Type"
-FROM 
-    df_participant sp
-JOIN 
-    df_study s ON sp."study.phs_accession" = s.phs_accession
-JOIN 
-    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-JOIN
-    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
-JOIN
-    df_program p ON p.program_acronym = s."program.program_acronym"
-JOIN
-    df_file f1 ON f1."sample.sample_id" = smp.sample_id
-JOIN
-    df_genomic_info gi ON gi."file.file_id" = f1.file_id
-WHERE 
-    s.phs_accession = 'phs001287' AND sp.gender = 'Female'
-ORDER BY 
-    smp.sample_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
-    f1.file_name AS "File Name",
-    s.study_name AS "Study Name",
-    s.phs_accession AS "Accession",
-    sp.participant_id AS "Participant Id",
-    COALESCE((
-        SELECT
-            REPLACE(GROUP_CONCAT(CASE WHEN rn &lt;= 5 THEN smp.sample_id ELSE NULL END, ', '), ', , ', ', ') ||
-            CASE WHEN MAX(rn) &gt; 5 THEN ', ...' ELSE '' END
-        FROM (
-            SELECT
-                smp.sample_id,
-                ROW_NUMBER() OVER (ORDER BY smp.sample_id) AS rn
-            FROM df_sample smp
-            WHERE smp."participant.study_participant_id" = sp.study_participant_id
-        ) smp
-    ), '') AS "Sample Id",
-    f1.file_type AS "File Type",
-    gi.library_strategy AS "Library Strategy"
-FROM 
-    df_study s
-INNER JOIN 
-    df_participant sp ON sp."study.phs_accession" = s.phs_accession
-INNER JOIN  
-    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-INNER JOIN 
-    df_file f1 ON f1."sample.sample_id" = smp.sample_id
-INNER JOIN
-    df_genomic_info gi ON gi."file.file_id" = f1.file_id
-INNER JOIN
-    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
-INNER JOIN
-    df_program p ON p.program_acronym = s."program.program_acronym"
-WHERE 
-    s.phs_accession = 'phs001287' AND sp.gender = 'Female'
-GROUP BY
-    f1.file_name,
-    s.study_name,
-    s.phs_accession,
-    sp.participant_id,
-    f1.file_type,
-    gi.library_strategy
-ORDER BY 
-    f1.file_name ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>TC02_CDS_phs002371_Gender_NotReported_TSVData.xlsx</t>
-  </si>
-  <si>
-    <t>TC02_CDS_phs002371_Gender_NotReported_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>SELECT
-    COUNT(DISTINCT s.study_name) AS "Studies",
-    COUNT(DISTINCT sp.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    COUNT(DISTINCT f.file_id) AS "Files"
-FROM 
-    df_participant sp
-JOIN 
-    df_study s ON sp."study.phs_accession" = s.phs_accession
-JOIN 
-    df_sample smp ON smp."participant.study_participant_id" = sp.study_participant_id
-JOIN 
-    df_program p ON p.program_acronym = s."program.program_acronym"
-JOIN 
-    df_file f ON f."sample.sample_id" = smp.sample_id
-JOIN 
-    df_diagnosis d ON d."participant.study_participant_id" = sp.study_participant_id
-JOIN 
-    df_genomic_info gi ON gi."file.file_id" = f.file_id
-WHERE 
-    s.phs_accession = 'phs002371' AND sp.gender = 'Female';</t>
   </si>
 </sst>
 </file>
@@ -611,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -645,16 +643,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
@@ -662,7 +660,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -671,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
     </row>

</xml_diff>